<commit_message>
multiple equal poles 8 set point
</commit_message>
<xml_diff>
--- a/Benchmark_System/MAX SENSITIVITY 1.4/Multiple Equal Poles 4/Multiple Equal Poles4_ms14.xlsx
+++ b/Benchmark_System/MAX SENSITIVITY 1.4/Multiple Equal Poles 4/Multiple Equal Poles4_ms14.xlsx
@@ -161,16 +161,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.3631908373345962</v>
+        <v>2.3631899612946223</v>
       </c>
       <c r="C2">
-        <v>3.8826738581970677</v>
+        <v>3.8824983095132808</v>
       </c>
       <c r="D2">
-        <v>3.6340581670202345</v>
+        <v>3.6330016612950375</v>
       </c>
       <c r="E2">
-        <v>2.6515051456752583</v>
+        <v>0.8255980946300262</v>
       </c>
     </row>
     <row r="3">
@@ -178,16 +178,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.3065978982991959</v>
+        <v>1.3066119353810981</v>
       </c>
       <c r="C3">
-        <v>5.2718000446242641</v>
+        <v>5.271465140788357</v>
       </c>
       <c r="D3">
-        <v>1.6201037069070972</v>
+        <v>1.6186022660001569</v>
       </c>
       <c r="E3">
-        <v>1.1065510872101187</v>
+        <v>5.0968846257258793</v>
       </c>
     </row>
     <row r="4">
@@ -195,16 +195,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2.7450290981344003</v>
+        <v>2.744953431473101</v>
       </c>
       <c r="C4">
-        <v>2.9950487675058035</v>
+        <v>2.9953444281333996</v>
       </c>
       <c r="D4">
-        <v>5.3469547349505815</v>
+        <v>5.3167672498780094</v>
       </c>
       <c r="E4">
-        <v>2.6939665193905213</v>
+        <v>3.9005271121602982</v>
       </c>
     </row>
     <row r="5">
@@ -212,16 +212,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1.1877325078533634</v>
+        <v>1.1878556071561832</v>
       </c>
       <c r="C5">
-        <v>1.2011076273330434</v>
+        <v>1.2007418807514199</v>
       </c>
       <c r="D5">
-        <v>1.9282849613260966</v>
+        <v>1.9279333932121985</v>
       </c>
       <c r="E5">
-        <v>1.0680656501999615</v>
+        <v>1.1867814052409109</v>
       </c>
     </row>
     <row r="6">
@@ -229,7 +229,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>6.2650076412046038</v>
+        <v>0.75087811552978445</v>
       </c>
     </row>
     <row r="7">
@@ -271,16 +271,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>121.39611288957357</v>
+        <v>121.3979561412464</v>
       </c>
       <c r="C9">
-        <v>102.89975751748455</v>
+        <v>103.65609784977876</v>
       </c>
       <c r="D9">
-        <v>116.06200089300495</v>
+        <v>117.09524216621371</v>
       </c>
       <c r="E9">
-        <v>9.7626988626210238</v>
+        <v>126.54394667475114</v>
       </c>
     </row>
     <row r="10">
@@ -288,7 +288,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>0.24780783691616323</v>
+        <v>25.601111440288133</v>
       </c>
     </row>
     <row r="11">
@@ -296,16 +296,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1.3999999986714806</v>
+        <v>1.3999999994566925</v>
       </c>
       <c r="C11">
-        <v>1.3999999391484594</v>
+        <v>1.3999998355699337</v>
       </c>
       <c r="D11">
-        <v>1.3999791846333813</v>
+        <v>1.3999786774595075</v>
       </c>
       <c r="E11">
-        <v>1.3999999843406841</v>
+        <v>1.3999979751247735</v>
       </c>
     </row>
     <row r="12">
@@ -313,16 +313,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2.764980145250008</v>
+        <v>2.7649400953948122</v>
       </c>
       <c r="C12">
-        <v>4.6610906930609541</v>
+        <v>4.6617607344072516</v>
       </c>
       <c r="D12">
-        <v>5.4412965241870541</v>
+        <v>5.4138478873375</v>
       </c>
       <c r="E12">
-        <v>3.1150478090410108</v>
+        <v>0.96754328040951476</v>
       </c>
     </row>
     <row r="13">
@@ -330,16 +330,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>11.391579621928555</v>
+        <v>11.392702095153142</v>
       </c>
       <c r="C13">
-        <v>13.088250948430279</v>
+        <v>13.08895253319049</v>
       </c>
       <c r="D13">
-        <v>8.8361710446392969</v>
+        <v>8.7790992131708077</v>
       </c>
       <c r="E13">
-        <v>5.5037325573174005</v>
+        <v>1.5023597780173634</v>
       </c>
     </row>
     <row r="14">
@@ -347,16 +347,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2.5443569954256118</v>
+        <v>2.5452977567500756</v>
       </c>
       <c r="C14">
-        <v>4.1035474928053484</v>
+        <v>4.1002052642163722</v>
       </c>
       <c r="D14">
-        <v>1.624843797901776</v>
+        <v>1.7025443527128425</v>
       </c>
       <c r="E14">
-        <v>1.9231829070385009</v>
+        <v>1.8395614034637076</v>
       </c>
     </row>
     <row r="15">
@@ -381,16 +381,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1.0254435699542561</v>
+        <v>1.0254529775675008</v>
       </c>
       <c r="C16">
-        <v>1.0410354749280535</v>
+        <v>1.0410020526421637</v>
       </c>
       <c r="D16">
-        <v>1.0162484379790189</v>
+        <v>1.0170254435271173</v>
       </c>
       <c r="E16">
-        <v>1.0192318290703848</v>
+        <v>1.0183956140346371</v>
       </c>
     </row>
     <row r="17">
@@ -398,16 +398,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>9.8010543900053637</v>
+        <v>9.8007749295388731</v>
       </c>
       <c r="C17">
-        <v>8.5488757122591856</v>
+        <v>8.545750363861643</v>
       </c>
       <c r="D17">
-        <v>14.249342208192667</v>
+        <v>14.164002362755896</v>
       </c>
       <c r="E17">
-        <v>10.526236214523214</v>
+        <v>1.9197927718678569</v>
       </c>
     </row>
     <row r="18">
@@ -415,16 +415,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>5.909554907170155</v>
+        <v>5.9094172135756997</v>
       </c>
       <c r="C18">
-        <v>3.7720766694191097</v>
+        <v>3.7710212715871574</v>
       </c>
       <c r="D18">
-        <v>3.6883587075379363</v>
+        <v>3.6890425452043223</v>
       </c>
       <c r="E18">
-        <v>5.3364719632357325</v>
+        <v>11.12240557975192</v>
       </c>
     </row>
     <row r="19">
@@ -432,16 +432,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>68.57693051601882</v>
+        <v>68.578349895128355</v>
       </c>
       <c r="C19">
-        <v>64.851724462827789</v>
+        <v>64.856945603168015</v>
       </c>
       <c r="D19">
-        <v>72.270921729841874</v>
+        <v>72.110912306016473</v>
       </c>
       <c r="E19">
-        <v>67.867805637871328</v>
+        <v>68.905032887965518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>